<commit_message>
Add DeviceConfig.xml to check devices available or not.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.10.10.10_GUIForDeviceStatusPolling.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.10.10.10_GUIForDeviceStatusPolling.xlsx
@@ -3955,7 +3955,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C:\\Automation-2014-11\\NformTestMain\\NformTester\\NformTester\\precondition_default.xml</t>
+    <t>C:\\Automation-2014-11\\NformTestMain\\NformTester\\NformTester\\precondition_license.xml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4496,7 +4496,7 @@
   <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>